<commit_message>
ipynb with weight process
</commit_message>
<xml_diff>
--- a/Model/htau.xlsx
+++ b/Model/htau.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1003" uniqueCount="1003">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1417" uniqueCount="1417">
   <si>
     <t>Var1_ 1</t>
   </si>
@@ -3022,6 +3022,1248 @@
   </si>
   <si>
     <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_27</t>
+  </si>
+  <si>
+    <t>Var1_28</t>
+  </si>
+  <si>
+    <t>Var1_29</t>
+  </si>
+  <si>
+    <t>Var1_30</t>
+  </si>
+  <si>
+    <t>Var1_31</t>
+  </si>
+  <si>
+    <t>Var1_32</t>
+  </si>
+  <si>
+    <t>Var1_33</t>
+  </si>
+  <si>
+    <t>Var1_34</t>
+  </si>
+  <si>
+    <t>Var1_35</t>
+  </si>
+  <si>
+    <t>Var1_36</t>
+  </si>
+  <si>
+    <t>Var1_37</t>
+  </si>
+  <si>
+    <t>Var1_38</t>
+  </si>
+  <si>
+    <t>Var1_39</t>
+  </si>
+  <si>
+    <t>Var1_40</t>
+  </si>
+  <si>
+    <t>Var1_41</t>
+  </si>
+  <si>
+    <t>Var1_42</t>
+  </si>
+  <si>
+    <t>Var1_43</t>
+  </si>
+  <si>
+    <t>Var1_44</t>
+  </si>
+  <si>
+    <t>Var1_45</t>
+  </si>
+  <si>
+    <t>Var1_46</t>
+  </si>
+  <si>
+    <t>Var1_47</t>
+  </si>
+  <si>
+    <t>Var1_48</t>
+  </si>
+  <si>
+    <t>Var1_49</t>
+  </si>
+  <si>
+    <t>Var1_50</t>
+  </si>
+  <si>
+    <t>Var1_51</t>
+  </si>
+  <si>
+    <t>Var1_ 1</t>
+  </si>
+  <si>
+    <t>Var1_ 2</t>
+  </si>
+  <si>
+    <t>Var1_ 3</t>
+  </si>
+  <si>
+    <t>Var1_ 4</t>
+  </si>
+  <si>
+    <t>Var1_ 5</t>
+  </si>
+  <si>
+    <t>Var1_ 6</t>
+  </si>
+  <si>
+    <t>Var1_ 7</t>
+  </si>
+  <si>
+    <t>Var1_ 8</t>
+  </si>
+  <si>
+    <t>Var1_ 9</t>
+  </si>
+  <si>
+    <t>Var1_10</t>
+  </si>
+  <si>
+    <t>Var1_11</t>
+  </si>
+  <si>
+    <t>Var1_12</t>
+  </si>
+  <si>
+    <t>Var1_13</t>
+  </si>
+  <si>
+    <t>Var1_14</t>
+  </si>
+  <si>
+    <t>Var1_15</t>
+  </si>
+  <si>
+    <t>Var1_16</t>
+  </si>
+  <si>
+    <t>Var1_17</t>
+  </si>
+  <si>
+    <t>Var1_18</t>
+  </si>
+  <si>
+    <t>Var1_19</t>
+  </si>
+  <si>
+    <t>Var1_20</t>
+  </si>
+  <si>
+    <t>Var1_21</t>
+  </si>
+  <si>
+    <t>Var1_22</t>
+  </si>
+  <si>
+    <t>Var1_23</t>
+  </si>
+  <si>
+    <t>Var1_24</t>
+  </si>
+  <si>
+    <t>Var1_25</t>
+  </si>
+  <si>
+    <t>Var1_26</t>
+  </si>
+  <si>
+    <t>Var1_27</t>
+  </si>
+  <si>
+    <t>Var1_28</t>
+  </si>
+  <si>
+    <t>Var1_29</t>
+  </si>
+  <si>
+    <t>Var1_30</t>
+  </si>
+  <si>
+    <t>Var1_31</t>
+  </si>
+  <si>
+    <t>Var1_32</t>
+  </si>
+  <si>
+    <t>Var1_33</t>
+  </si>
+  <si>
+    <t>Var1_34</t>
+  </si>
+  <si>
+    <t>Var1_35</t>
+  </si>
+  <si>
+    <t>Var1_36</t>
+  </si>
+  <si>
+    <t>Var1_37</t>
+  </si>
+  <si>
+    <t>Var1_38</t>
+  </si>
+  <si>
+    <t>Var1_39</t>
+  </si>
+  <si>
+    <t>Var1_40</t>
+  </si>
+  <si>
+    <t>Var1_41</t>
+  </si>
+  <si>
+    <t>Var1_42</t>
+  </si>
+  <si>
+    <t>Var1_43</t>
+  </si>
+  <si>
+    <t>Var1_44</t>
+  </si>
+  <si>
+    <t>Var1_45</t>
+  </si>
+  <si>
+    <t>Var1_46</t>
+  </si>
+  <si>
+    <t>Var1_47</t>
+  </si>
+  <si>
+    <t>Var1_48</t>
+  </si>
+  <si>
+    <t>Var1_49</t>
+  </si>
+  <si>
+    <t>Var1_50</t>
+  </si>
+  <si>
+    <t>Var1_51</t>
   </si>
 </sst>
 </file>
@@ -3042,7 +4284,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="29">
+  <borders count="43">
     <border>
       <left/>
       <right/>
@@ -3078,11 +4320,25 @@
     <border/>
     <border/>
     <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="true"/>
@@ -3112,6 +4368,20 @@
     <xf numFmtId="22" fontId="0" fillId="0" borderId="26" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="27" xfId="0" applyNumberFormat="true"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="28" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="29" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="30" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="31" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="32" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="33" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="34" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="35" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="36" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="37" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="38" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="39" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="40" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="41" xfId="0" applyNumberFormat="true"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="42" xfId="0" applyNumberFormat="true"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -3124,522 +4394,522 @@
   <dimension ref="A1:AY3"/>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="14.7109375" customWidth="true"/>
-    <col min="2" max="2" width="14.7109375" customWidth="true"/>
-    <col min="3" max="3" width="15.7109375" customWidth="true"/>
-    <col min="4" max="4" width="15.34765625" customWidth="true"/>
-    <col min="5" max="5" width="15.34765625" customWidth="true"/>
-    <col min="6" max="6" width="15.34765625" customWidth="true"/>
-    <col min="7" max="7" width="15.34765625" customWidth="true"/>
-    <col min="8" max="8" width="14.34765625" customWidth="true"/>
+    <col min="1" max="1" width="15.7109375" customWidth="true"/>
+    <col min="2" max="2" width="15.7109375" customWidth="true"/>
+    <col min="3" max="3" width="14.7109375" customWidth="true"/>
+    <col min="4" max="4" width="15.7109375" customWidth="true"/>
+    <col min="5" max="5" width="15.7109375" customWidth="true"/>
+    <col min="6" max="6" width="14.7109375" customWidth="true"/>
+    <col min="7" max="7" width="15.7109375" customWidth="true"/>
+    <col min="8" max="8" width="15.7109375" customWidth="true"/>
     <col min="9" max="9" width="15.7109375" customWidth="true"/>
     <col min="10" max="10" width="15.7109375" customWidth="true"/>
     <col min="11" max="11" width="15.7109375" customWidth="true"/>
-    <col min="12" max="12" width="14.7109375" customWidth="true"/>
-    <col min="13" max="13" width="13.7109375" customWidth="true"/>
-    <col min="14" max="14" width="14.7109375" customWidth="true"/>
+    <col min="12" max="12" width="15.7109375" customWidth="true"/>
+    <col min="13" max="13" width="15.7109375" customWidth="true"/>
+    <col min="14" max="14" width="15.7109375" customWidth="true"/>
     <col min="15" max="15" width="14.7109375" customWidth="true"/>
-    <col min="16" max="16" width="14.7109375" customWidth="true"/>
-    <col min="17" max="17" width="14.7109375" customWidth="true"/>
-    <col min="18" max="18" width="13.7109375" customWidth="true"/>
+    <col min="16" max="16" width="15.7109375" customWidth="true"/>
+    <col min="17" max="17" width="15.7109375" customWidth="true"/>
+    <col min="18" max="18" width="15.7109375" customWidth="true"/>
     <col min="19" max="19" width="15.7109375" customWidth="true"/>
     <col min="20" max="20" width="15.7109375" customWidth="true"/>
     <col min="21" max="21" width="15.7109375" customWidth="true"/>
-    <col min="22" max="22" width="15.7109375" customWidth="true"/>
+    <col min="22" max="22" width="14.7109375" customWidth="true"/>
     <col min="23" max="23" width="15.7109375" customWidth="true"/>
-    <col min="24" max="24" width="15.34765625" customWidth="true"/>
-    <col min="25" max="25" width="15.34765625" customWidth="true"/>
-    <col min="26" max="26" width="15.34765625" customWidth="true"/>
-    <col min="27" max="27" width="15.34765625" customWidth="true"/>
-    <col min="28" max="28" width="15.34765625" customWidth="true"/>
-    <col min="29" max="29" width="15.34765625" customWidth="true"/>
-    <col min="30" max="30" width="15.34765625" customWidth="true"/>
-    <col min="31" max="31" width="15.34765625" customWidth="true"/>
-    <col min="32" max="32" width="15.34765625" customWidth="true"/>
-    <col min="33" max="33" width="15.34765625" customWidth="true"/>
-    <col min="34" max="34" width="15.34765625" customWidth="true"/>
-    <col min="35" max="35" width="15.34765625" customWidth="true"/>
-    <col min="36" max="36" width="15.34765625" customWidth="true"/>
-    <col min="37" max="37" width="15.34765625" customWidth="true"/>
-    <col min="38" max="38" width="15.34765625" customWidth="true"/>
-    <col min="39" max="39" width="15.34765625" customWidth="true"/>
-    <col min="40" max="40" width="15.34765625" customWidth="true"/>
-    <col min="41" max="41" width="15.34765625" customWidth="true"/>
-    <col min="42" max="42" width="15.34765625" customWidth="true"/>
-    <col min="43" max="43" width="15.34765625" customWidth="true"/>
-    <col min="44" max="44" width="13.34765625" customWidth="true"/>
-    <col min="45" max="45" width="15.34765625" customWidth="true"/>
-    <col min="46" max="46" width="15.34765625" customWidth="true"/>
-    <col min="47" max="47" width="15.34765625" customWidth="true"/>
-    <col min="48" max="48" width="15.34765625" customWidth="true"/>
-    <col min="49" max="49" width="15.34765625" customWidth="true"/>
-    <col min="50" max="50" width="15.34765625" customWidth="true"/>
+    <col min="24" max="24" width="15.7109375" customWidth="true"/>
+    <col min="25" max="25" width="15.7109375" customWidth="true"/>
+    <col min="26" max="26" width="15.7109375" customWidth="true"/>
+    <col min="27" max="27" width="15.7109375" customWidth="true"/>
+    <col min="28" max="28" width="15.7109375" customWidth="true"/>
+    <col min="29" max="29" width="15.7109375" customWidth="true"/>
+    <col min="30" max="30" width="15.7109375" customWidth="true"/>
+    <col min="31" max="31" width="14.7109375" customWidth="true"/>
+    <col min="32" max="32" width="14.7109375" customWidth="true"/>
+    <col min="33" max="33" width="15.7109375" customWidth="true"/>
+    <col min="34" max="34" width="15.7109375" customWidth="true"/>
+    <col min="35" max="35" width="15.7109375" customWidth="true"/>
+    <col min="36" max="36" width="15.7109375" customWidth="true"/>
+    <col min="37" max="37" width="15.7109375" customWidth="true"/>
+    <col min="38" max="38" width="15.7109375" customWidth="true"/>
+    <col min="39" max="39" width="14.7109375" customWidth="true"/>
+    <col min="40" max="40" width="15.7109375" customWidth="true"/>
+    <col min="41" max="41" width="15.7109375" customWidth="true"/>
+    <col min="42" max="42" width="15.7109375" customWidth="true"/>
+    <col min="43" max="43" width="15.7109375" customWidth="true"/>
+    <col min="44" max="44" width="15.7109375" customWidth="true"/>
+    <col min="45" max="45" width="15.7109375" customWidth="true"/>
+    <col min="46" max="46" width="14.7109375" customWidth="true"/>
+    <col min="47" max="47" width="15.7109375" customWidth="true"/>
+    <col min="48" max="48" width="14.7109375" customWidth="true"/>
+    <col min="49" max="49" width="15.7109375" customWidth="true"/>
+    <col min="50" max="50" width="15.7109375" customWidth="true"/>
     <col min="51" max="51" width="15.34765625" customWidth="true"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" s="0" t="s">
-        <v>977</v>
+        <v>1366</v>
       </c>
       <c r="B1" s="0" t="s">
-        <v>978</v>
+        <v>1367</v>
       </c>
       <c r="C1" s="0" t="s">
-        <v>979</v>
+        <v>1368</v>
       </c>
       <c r="D1" s="0" t="s">
-        <v>980</v>
+        <v>1369</v>
       </c>
       <c r="E1" s="0" t="s">
-        <v>981</v>
+        <v>1370</v>
       </c>
       <c r="F1" s="0" t="s">
-        <v>982</v>
+        <v>1371</v>
       </c>
       <c r="G1" s="0" t="s">
-        <v>983</v>
+        <v>1372</v>
       </c>
       <c r="H1" s="0" t="s">
-        <v>984</v>
+        <v>1373</v>
       </c>
       <c r="I1" s="0" t="s">
-        <v>985</v>
+        <v>1374</v>
       </c>
       <c r="J1" s="0" t="s">
-        <v>986</v>
+        <v>1375</v>
       </c>
       <c r="K1" s="0" t="s">
-        <v>987</v>
+        <v>1376</v>
       </c>
       <c r="L1" s="0" t="s">
-        <v>988</v>
+        <v>1377</v>
       </c>
       <c r="M1" s="0" t="s">
-        <v>989</v>
+        <v>1378</v>
       </c>
       <c r="N1" s="0" t="s">
-        <v>990</v>
+        <v>1379</v>
       </c>
       <c r="O1" s="0" t="s">
-        <v>991</v>
+        <v>1380</v>
       </c>
       <c r="P1" s="0" t="s">
-        <v>992</v>
+        <v>1381</v>
       </c>
       <c r="Q1" s="0" t="s">
-        <v>993</v>
+        <v>1382</v>
       </c>
       <c r="R1" s="0" t="s">
-        <v>994</v>
+        <v>1383</v>
       </c>
       <c r="S1" s="0" t="s">
-        <v>995</v>
+        <v>1384</v>
       </c>
       <c r="T1" s="0" t="s">
-        <v>996</v>
+        <v>1385</v>
       </c>
       <c r="U1" s="0" t="s">
-        <v>997</v>
+        <v>1386</v>
       </c>
       <c r="V1" s="0" t="s">
-        <v>998</v>
+        <v>1387</v>
       </c>
       <c r="W1" s="0" t="s">
-        <v>999</v>
+        <v>1388</v>
       </c>
       <c r="X1" s="0" t="s">
-        <v>1000</v>
+        <v>1389</v>
       </c>
       <c r="Y1" s="0" t="s">
-        <v>1001</v>
+        <v>1390</v>
       </c>
       <c r="Z1" s="0" t="s">
-        <v>1002</v>
+        <v>1391</v>
       </c>
       <c r="AA1" s="0" t="s">
-        <v>614</v>
+        <v>1392</v>
       </c>
       <c r="AB1" s="0" t="s">
-        <v>615</v>
+        <v>1393</v>
       </c>
       <c r="AC1" s="0" t="s">
-        <v>616</v>
+        <v>1394</v>
       </c>
       <c r="AD1" s="0" t="s">
-        <v>617</v>
+        <v>1395</v>
       </c>
       <c r="AE1" s="0" t="s">
-        <v>618</v>
+        <v>1396</v>
       </c>
       <c r="AF1" s="0" t="s">
-        <v>619</v>
+        <v>1397</v>
       </c>
       <c r="AG1" s="0" t="s">
-        <v>620</v>
+        <v>1398</v>
       </c>
       <c r="AH1" s="0" t="s">
-        <v>621</v>
+        <v>1399</v>
       </c>
       <c r="AI1" s="0" t="s">
-        <v>622</v>
+        <v>1400</v>
       </c>
       <c r="AJ1" s="0" t="s">
-        <v>623</v>
+        <v>1401</v>
       </c>
       <c r="AK1" s="0" t="s">
-        <v>624</v>
+        <v>1402</v>
       </c>
       <c r="AL1" s="0" t="s">
-        <v>625</v>
+        <v>1403</v>
       </c>
       <c r="AM1" s="0" t="s">
-        <v>626</v>
+        <v>1404</v>
       </c>
       <c r="AN1" s="0" t="s">
-        <v>627</v>
+        <v>1405</v>
       </c>
       <c r="AO1" s="0" t="s">
-        <v>628</v>
+        <v>1406</v>
       </c>
       <c r="AP1" s="0" t="s">
-        <v>629</v>
+        <v>1407</v>
       </c>
       <c r="AQ1" s="0" t="s">
-        <v>630</v>
+        <v>1408</v>
       </c>
       <c r="AR1" s="0" t="s">
-        <v>631</v>
+        <v>1409</v>
       </c>
       <c r="AS1" s="0" t="s">
-        <v>632</v>
+        <v>1410</v>
       </c>
       <c r="AT1" s="0" t="s">
-        <v>633</v>
+        <v>1411</v>
       </c>
       <c r="AU1" s="0" t="s">
-        <v>634</v>
+        <v>1412</v>
       </c>
       <c r="AV1" s="0" t="s">
-        <v>635</v>
+        <v>1413</v>
       </c>
       <c r="AW1" s="0" t="s">
-        <v>636</v>
+        <v>1414</v>
       </c>
       <c r="AX1" s="0" t="s">
-        <v>637</v>
+        <v>1415</v>
       </c>
       <c r="AY1" s="0" t="s">
-        <v>638</v>
+        <v>1416</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="0">
-        <v>0.0044630323880127951</v>
+        <v>0.00020002652839335171</v>
       </c>
       <c r="B2" s="0">
-        <v>0.00075430908797727183</v>
+        <v>0.00019912791974267249</v>
       </c>
       <c r="C2" s="0">
-        <v>0.00019653307341911897</v>
+        <v>0.00019900713901439999</v>
       </c>
       <c r="D2" s="0">
-        <v>9.5385670953992651e-05</v>
+        <v>0.00019901529481972612</v>
       </c>
       <c r="E2" s="0">
-        <v>6.6704488809508499e-05</v>
+        <v>0.00019911415893363214</v>
       </c>
       <c r="F2" s="0">
-        <v>4.7887087441314942e-05</v>
+        <v>0.00019940969200106805</v>
       </c>
       <c r="G2" s="0">
-        <v>3.5353154410456614e-05</v>
+        <v>0.00020021130806929815</v>
       </c>
       <c r="H2" s="0">
-        <v>6.3603947504787758e-05</v>
+        <v>0.00020215600964480562</v>
       </c>
       <c r="I2" s="0">
-        <v>0.00013781160185390208</v>
+        <v>0.00020636667629332227</v>
       </c>
       <c r="J2" s="0">
-        <v>0.00031233090270957364</v>
+        <v>0.00021442311917747642</v>
       </c>
       <c r="K2" s="0">
-        <v>0.00061083653143252138</v>
+        <v>0.00022787162784040907</v>
       </c>
       <c r="L2" s="0">
-        <v>0.001062787121829475</v>
+        <v>0.00024717015388762043</v>
       </c>
       <c r="M2" s="0">
-        <v>0.0015660227302353742</v>
+        <v>0.00027073818647689303</v>
       </c>
       <c r="N2" s="0">
-        <v>0.0016137108553368508</v>
+        <v>0.00029435013262289604</v>
       </c>
       <c r="O2" s="0">
-        <v>0.0015701984306006086</v>
+        <v>0.0003021110120151522</v>
       </c>
       <c r="P2" s="0">
-        <v>0.0016096808986298399</v>
+        <v>0.00029966046673562225</v>
       </c>
       <c r="Q2" s="0">
-        <v>0.001433616397454033</v>
+        <v>0.00028567223110167312</v>
       </c>
       <c r="R2" s="0">
-        <v>0.0016123782899559918</v>
+        <v>0.00026573797261377407</v>
       </c>
       <c r="S2" s="0">
-        <v>0.00096156302874173623</v>
+        <v>0.00024969389082602357</v>
       </c>
       <c r="T2" s="0">
-        <v>0.00065826083757591892</v>
+        <v>0.00023024893020599343</v>
       </c>
       <c r="U2" s="0">
-        <v>0.00047536615317768241</v>
+        <v>0.00021811808422346962</v>
       </c>
       <c r="V2" s="0">
-        <v>0.000294906170820005</v>
+        <v>0.00021064402204856367</v>
       </c>
       <c r="W2" s="0">
-        <v>0.00016859083972749325</v>
+        <v>0.0002060719641768035</v>
       </c>
       <c r="X2" s="0">
-        <v>9.3869872808636338e-05</v>
+        <v>0.00020328568157753607</v>
       </c>
       <c r="Y2" s="0">
-        <v>3.7836387270208477e-05</v>
+        <v>0.00020085561430588614</v>
       </c>
       <c r="Z2" s="0">
-        <v>1.4534032544816511e-05</v>
+        <v>0.00057041408936459091</v>
       </c>
       <c r="AA2" s="0">
-        <v>4.4194232022479084e-06</v>
+        <v>0.00018345168547193955</v>
       </c>
       <c r="AB2" s="0">
-        <v>3.9796029951750495e-06</v>
+        <v>0.00013920696180341787</v>
       </c>
       <c r="AC2" s="0">
-        <v>3.7059799165774996e-06</v>
+        <v>0.0001339315421114149</v>
       </c>
       <c r="AD2" s="0">
-        <v>3.5358301576377244e-06</v>
+        <v>0.00013326103681507993</v>
       </c>
       <c r="AE2" s="0">
-        <v>3.4300213426319432e-06</v>
+        <v>0.00013316734096984736</v>
       </c>
       <c r="AF2" s="0">
-        <v>3.3642222692036374e-06</v>
+        <v>0.00013316189297604982</v>
       </c>
       <c r="AG2" s="0">
-        <v>3.3233035231603054e-06</v>
+        <v>0.00013319659836301363</v>
       </c>
       <c r="AH2" s="0">
-        <v>3.2978570427645599e-06</v>
+        <v>0.00013329893462304325</v>
       </c>
       <c r="AI2" s="0">
-        <v>3.2820323637202362e-06</v>
+        <v>0.00013357712766484279</v>
       </c>
       <c r="AJ2" s="0">
-        <v>3.2721912736232593e-06</v>
+        <v>0.00013425471920425173</v>
       </c>
       <c r="AK2" s="0">
-        <v>3.266071262734193e-06</v>
+        <v>0.00013574208967268277</v>
       </c>
       <c r="AL2" s="0">
-        <v>3.2622653255975771e-06</v>
+        <v>0.00013866135984957019</v>
       </c>
       <c r="AM2" s="0">
-        <v>3.2598984725567898e-06</v>
+        <v>0.00014373683402974863</v>
       </c>
       <c r="AN2" s="0">
-        <v>3.25842656294431e-06</v>
+        <v>0.0001514705888507877</v>
       </c>
       <c r="AO2" s="0">
-        <v>3.2575112047093576e-06</v>
+        <v>0.0001617281073927069</v>
       </c>
       <c r="AP2" s="0">
-        <v>3.2569419572399938e-06</v>
+        <v>0.00017373140863844198</v>
       </c>
       <c r="AQ2" s="0">
-        <v>3.2565879507988393e-06</v>
+        <v>0.00018662996746081714</v>
       </c>
       <c r="AR2" s="0">
-        <v>3.2563677995038733e-06</v>
+        <v>0.00019868130114234801</v>
       </c>
       <c r="AS2" s="0">
-        <v>3.2562308907113703e-06</v>
+        <v>0.00020388841562413081</v>
       </c>
       <c r="AT2" s="0">
-        <v>3.2561457491823072e-06</v>
+        <v>0.00019427531903322781</v>
       </c>
       <c r="AU2" s="0">
-        <v>3.2560928009388943e-06</v>
+        <v>0.00017448185775972901</v>
       </c>
       <c r="AV2" s="0">
-        <v>3.2560598732180124e-06</v>
+        <v>0.00015817082402706041</v>
       </c>
       <c r="AW2" s="0">
-        <v>3.2560393959606316e-06</v>
+        <v>0.00014837095958655184</v>
       </c>
       <c r="AX2" s="0">
-        <v>3.2560266614603381e-06</v>
+        <v>0.0001395027373930806</v>
       </c>
       <c r="AY2" s="0">
-        <v>1.3024022868190929e-07</v>
+        <v>3.9582956762821524e-09</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0">
-        <v>0.0066270093148288033</v>
+        <v>0.00033569889768528</v>
       </c>
       <c r="B3" s="0">
-        <v>3.4293470420985469e-05</v>
+        <v>0.00033569889768054052</v>
       </c>
       <c r="C3" s="0">
-        <v>1.4758593765515126e-07</v>
+        <v>0.0003356988976805152</v>
       </c>
       <c r="D3" s="0">
-        <v>2.6171499003138184e-09</v>
+        <v>0.00033569889768051504</v>
       </c>
       <c r="E3" s="0">
-        <v>2.2767386321984104e-09</v>
+        <v>0.00033569889768051829</v>
       </c>
       <c r="F3" s="0">
-        <v>2.3642427923456773e-09</v>
+        <v>0.00033569889768077102</v>
       </c>
       <c r="G3" s="0">
-        <v>2.6028477971453134e-09</v>
+        <v>0.00033569889769616507</v>
       </c>
       <c r="H3" s="0">
-        <v>2.214159787738172e-09</v>
+        <v>0.0003356988983976597</v>
       </c>
       <c r="I3" s="0">
-        <v>1.6342300056224501e-09</v>
+        <v>0.00033569892202526652</v>
       </c>
       <c r="J3" s="0">
-        <v>1.7461158009954448e-08</v>
+        <v>0.00033569950037143663</v>
       </c>
       <c r="K3" s="0">
-        <v>3.3182041577964553e-07</v>
+        <v>0.00033570959113212828</v>
       </c>
       <c r="L3" s="0">
-        <v>4.6737461103891714e-06</v>
+        <v>0.00033583236030762704</v>
       </c>
       <c r="M3" s="0">
-        <v>3.9587934646935556e-05</v>
+        <v>0.00033684779433910917</v>
       </c>
       <c r="N3" s="0">
-        <v>0.00011135800088172236</v>
+        <v>0.00034237338809941793</v>
       </c>
       <c r="O3" s="0">
-        <v>0.0002396748655402354</v>
+        <v>0.00035516693793706284</v>
       </c>
       <c r="P3" s="0">
-        <v>0.00064318068250807667</v>
+        <v>0.00037541835804734311</v>
       </c>
       <c r="Q3" s="0">
-        <v>0.00089849178259660337</v>
+        <v>0.00039529193772323503</v>
       </c>
       <c r="R3" s="0">
-        <v>0.003483428232555142</v>
+        <v>0.00039230254124255064</v>
       </c>
       <c r="S3" s="0">
-        <v>0.002003544016302026</v>
+        <v>0.00040195069629313457</v>
       </c>
       <c r="T3" s="0">
-        <v>0.0018050447513132438</v>
+        <v>0.00037750145024228446</v>
       </c>
       <c r="U3" s="0">
-        <v>0.0018789293926490046</v>
+        <v>0.00036162600971928103</v>
       </c>
       <c r="V3" s="0">
-        <v>0.0012043861945425264</v>
+        <v>0.00035162317074526891</v>
       </c>
       <c r="W3" s="0">
-        <v>0.00059900509480465057</v>
+        <v>0.00034543322908772955</v>
       </c>
       <c r="X3" s="0">
-        <v>0.00027771644429370622</v>
+        <v>0.00034163357060780351</v>
       </c>
       <c r="Y3" s="0">
-        <v>9.507681852098551e-05</v>
+        <v>0.00033931774904920429</v>
       </c>
       <c r="Z3" s="0">
-        <v>1.9046470262151153e-08</v>
+        <v>3.6474765399118255e-05</v>
       </c>
       <c r="AA3" s="0">
-        <v>1.7757475697789661e-13</v>
+        <v>3.6335389939167202e-05</v>
       </c>
       <c r="AB3" s="0">
-        <v>1.5967345967447567e-13</v>
+        <v>3.6334842539154324e-05</v>
       </c>
       <c r="AC3" s="0">
-        <v>1.4854091038996769e-13</v>
+        <v>3.6334840090933709e-05</v>
       </c>
       <c r="AD3" s="0">
-        <v>1.4161774434959009e-13</v>
+        <v>3.6334840077861572e-05</v>
       </c>
       <c r="AE3" s="0">
-        <v>1.3731233084566136e-13</v>
+        <v>3.6334840077776868e-05</v>
       </c>
       <c r="AF3" s="0">
-        <v>1.3463485852566851e-13</v>
+        <v>3.6334840077776191e-05</v>
       </c>
       <c r="AG3" s="0">
-        <v>1.3296977850076738e-13</v>
+        <v>3.6334840077776909e-05</v>
       </c>
       <c r="AH3" s="0">
-        <v>1.3193429011546369e-13</v>
+        <v>3.6334840077831078e-05</v>
       </c>
       <c r="AI3" s="0">
-        <v>1.312903353625002e-13</v>
+        <v>3.6334840080903782e-05</v>
       </c>
       <c r="AJ3" s="0">
-        <v>1.3088986952459268e-13</v>
+        <v>3.6334840214002507e-05</v>
       </c>
       <c r="AK3" s="0">
-        <v>1.3064082580437328e-13</v>
+        <v>3.633484457738481e-05</v>
       </c>
       <c r="AL3" s="0">
-        <v>1.3048594923636237e-13</v>
+        <v>3.633495136213683e-05</v>
       </c>
       <c r="AM3" s="0">
-        <v>1.3038963381311985e-13</v>
+        <v>3.63368732661106e-05</v>
       </c>
       <c r="AN3" s="0">
-        <v>1.3032973669069819e-13</v>
+        <v>3.6361902658477539e-05</v>
       </c>
       <c r="AO3" s="0">
-        <v>1.3029248756533893e-13</v>
+        <v>3.6593465506550238e-05</v>
       </c>
       <c r="AP3" s="0">
-        <v>1.3026932289091158e-13</v>
+        <v>3.808384872261919e-05</v>
       </c>
       <c r="AQ3" s="0">
-        <v>1.3025491712604734e-13</v>
+        <v>4.4618485716701599e-05</v>
       </c>
       <c r="AR3" s="0">
-        <v>1.3024595839615136e-13</v>
+        <v>6.3667759672678915e-05</v>
       </c>
       <c r="AS3" s="0">
-        <v>1.302403870959041e-13</v>
+        <v>9.7893489097315199e-05</v>
       </c>
       <c r="AT3" s="0">
-        <v>1.3023692238753527e-13</v>
+        <v>0.00012483962364519534</v>
       </c>
       <c r="AU3" s="0">
-        <v>1.302347677371757e-13</v>
+        <v>0.00010934776257906045</v>
       </c>
       <c r="AV3" s="0">
-        <v>1.3023342779231514e-13</v>
+        <v>7.9208254814172331e-05</v>
       </c>
       <c r="AW3" s="0">
-        <v>1.3023259450062988e-13</v>
+        <v>6.1881488851494237e-05</v>
       </c>
       <c r="AX3" s="0">
-        <v>1.3023207628898315e-13</v>
+        <v>5.1558240076174167e-05</v>
       </c>
       <c r="AY3" s="0">
-        <v>5.2092489594839171e-15</v>
+        <v>9.7172616021966786e-19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>